<commit_message>
Update hlr for standard user.xlsx
</commit_message>
<xml_diff>
--- a/Extra Work/hlr for standard user.xlsx
+++ b/Extra Work/hlr for standard user.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="192">
   <si>
     <t>functionality id</t>
   </si>
@@ -695,6 +695,18 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1DbwL26elHVJX2a9gQjG5iZ2WETe121ON/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1pEoLGI23P4U2gYL0PslUmoLH1BAeP_Q1/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1gQVo5aKPoCBtD9Uy23_07C8kcpZUu-aO/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1DlNEPMKd6O0Gj453c9VQnNaehj7pHxOR/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1j-VDGXnzhtUdogdJxWvctwo9wZAd0Dz8/view?usp=share_link</t>
   </si>
 </sst>
 </file>
@@ -3787,8 +3799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4458,7 +4470,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="7" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
         <v>18</v>
       </c>
@@ -4474,9 +4486,15 @@
       <c r="E17" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="F17" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>170</v>
+      </c>
       <c r="I17" s="24" t="s">
         <v>114</v>
       </c>
@@ -4486,12 +4504,14 @@
       <c r="K17" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="L17" s="24"/>
+      <c r="L17" s="36" t="s">
+        <v>188</v>
+      </c>
       <c r="M17" s="21" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <v>28</v>
       </c>
@@ -4507,9 +4527,15 @@
       <c r="E18" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="F18" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>169</v>
+      </c>
       <c r="I18" s="24" t="s">
         <v>128</v>
       </c>
@@ -4519,12 +4545,14 @@
       <c r="K18" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="L18" s="24"/>
+      <c r="L18" s="36" t="s">
+        <v>189</v>
+      </c>
       <c r="M18" s="21" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="24">
         <v>30</v>
       </c>
@@ -4540,9 +4568,15 @@
       <c r="E19" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="F19" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>171</v>
+      </c>
       <c r="I19" s="24" t="s">
         <v>132</v>
       </c>
@@ -4552,12 +4586,14 @@
       <c r="K19" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="L19" s="24"/>
+      <c r="L19" s="36" t="s">
+        <v>190</v>
+      </c>
       <c r="M19" s="21" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
         <v>33</v>
       </c>
@@ -4573,9 +4609,15 @@
       <c r="E20" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="F20" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>171</v>
+      </c>
       <c r="I20" s="24" t="s">
         <v>139</v>
       </c>
@@ -4585,7 +4627,9 @@
       <c r="K20" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="L20" s="24"/>
+      <c r="L20" s="36" t="s">
+        <v>191</v>
+      </c>
       <c r="M20" s="21" t="s">
         <v>167</v>
       </c>
@@ -4607,9 +4651,13 @@
     <hyperlink ref="L14" r:id="rId13"/>
     <hyperlink ref="L15" r:id="rId14"/>
     <hyperlink ref="L16" r:id="rId15"/>
+    <hyperlink ref="L17" r:id="rId16"/>
+    <hyperlink ref="L18" r:id="rId17"/>
+    <hyperlink ref="L19" r:id="rId18"/>
+    <hyperlink ref="L20" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>